<commit_message>
Updated testcases for NCATS Study multifilter
</commit_message>
<xml_diff>
--- a/InputFiles/TC02_Canine_StudyNCATSCOP01-StudyType_Biobank_StudyPart.xlsx
+++ b/InputFiles/TC02_Canine_StudyNCATSCOP01-StudyType_Biobank_StudyPart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davids3\newclone\sofia0302\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{851DDCAA-E9DA-4F8D-8903-AE79D955A61B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2453337-B53F-44F2-816E-6076CCAE3E58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -580,7 +580,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.3"/>

</xml_diff>